<commit_message>
Eliminate Some Scrutinizer 'Major' Problems Part 5
More of the same. 2 or 3 of these still to go after this.

Note one deprecation. Shared/Drawing has a method imagecreatefrombmp. However, that was introduced as a native PHP function with 7.2, so the method is no longer needed.
</commit_message>
<xml_diff>
--- a/samples/templates/27template.xlsx
+++ b/samples/templates/27template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\issue1482\samples\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\scrutmajor5\samples\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA4B681-FEEE-448D-9E0B-26C0A80F779C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEB3D61-B840-4905-9037-20FD607273FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,94 +326,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Billede 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E17F831F-95E3-03A1-8662-6B6A1703815B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="628650" y="400050"/>
-          <a:ext cx="1962150" cy="1377950"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:blipFill dpi="0" rotWithShape="0">
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-                <a:srcRect/>
-                <a:stretch>
-                  <a:fillRect/>
-                </a:stretch>
-              </a:blipFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cap="flat">
-              <a:solidFill>
-                <a:srgbClr val="3465A4"/>
-              </a:solidFill>
-              <a:round/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -439,7 +351,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -527,7 +439,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -615,7 +527,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -672,6 +584,56 @@
             </a14:hiddenEffects>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8700761F-13F9-D673-A870-B8D5F2E91CEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="400050"/>
+          <a:ext cx="1552575" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1064,7 +1026,7 @@
   <dimension ref="B2:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1084,6 +1046,7 @@
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Eliminate Some Scrutinizer 'Major' Problems Part 5 (#3161)
* Eliminate Some Scrutinizer 'Major' Problems Part 5

More of the same. 2 or 3 of these still to go after this.

Note one deprecation. Shared/Drawing has a method imagecreatefrombmp. However, that was introduced as a native PHP function with 7.2, so the method is no longer needed.

* More Silliness

Keep trying.

* If At First You Don't Succeed

Try, try again.
</commit_message>
<xml_diff>
--- a/samples/templates/27template.xlsx
+++ b/samples/templates/27template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\issue1482\samples\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\scrutmajor5\samples\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA4B681-FEEE-448D-9E0B-26C0A80F779C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEB3D61-B840-4905-9037-20FD607273FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,94 +326,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Billede 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E17F831F-95E3-03A1-8662-6B6A1703815B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="628650" y="400050"/>
-          <a:ext cx="1962150" cy="1377950"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:blipFill dpi="0" rotWithShape="0">
-                <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-                <a:srcRect/>
-                <a:stretch>
-                  <a:fillRect/>
-                </a:stretch>
-              </a:blipFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cap="flat">
-              <a:solidFill>
-                <a:srgbClr val="3465A4"/>
-              </a:solidFill>
-              <a:round/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -439,7 +351,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -527,7 +439,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -615,7 +527,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -672,6 +584,56 @@
             </a14:hiddenEffects>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8700761F-13F9-D673-A870-B8D5F2E91CEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="400050"/>
+          <a:ext cx="1552575" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1064,7 +1026,7 @@
   <dimension ref="B2:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1084,6 +1046,7 @@
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>